<commit_message>
Search, Date , Export added
</commit_message>
<xml_diff>
--- a/SellerPoint/SellerPoint/wwwroot/DealerSales.xlsx
+++ b/SellerPoint/SellerPoint/wwwroot/DealerSales.xlsx
@@ -12,15 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>Dealer</t>
+    <t>Created Date</t>
   </si>
   <si>
-    <t>Unit Price</t>
-  </si>
-  <si>
-    <t>Discount</t>
+    <t>Order No</t>
   </si>
   <si>
     <t>Payable Total</t>
@@ -29,16 +26,28 @@
     <t>Due</t>
   </si>
   <si>
-    <t>Order No</t>
+    <t>Dealer Name</t>
+  </si>
+  <si>
+    <t>S-0000001-130420-000000001</t>
   </si>
   <si>
     <t>Hasan</t>
   </si>
   <si>
-    <t>S-000001-090420-00000001</t>
+    <t>S-0000002-130420-000000002</t>
   </si>
   <si>
-    <t>S-000002-090420-00000002</t>
+    <t>Jewel</t>
+  </si>
+  <si>
+    <t>S-0000003-130420-000000003</t>
+  </si>
+  <si>
+    <t>Saad</t>
+  </si>
+  <si>
+    <t>S-0000004-130420-000000004</t>
   </si>
 </sst>
 </file>
@@ -84,7 +93,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -106,62 +115,73 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>0</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="0">
-        <v>100</v>
+      <c r="C2" s="0">
+        <v>4500</v>
       </c>
       <c r="D2" s="0">
-        <v>200</v>
+        <v>500</v>
       </c>
-      <c r="E2" s="0">
-        <v>100</v>
+      <c r="E2" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="s">
-        <v>6</v>
+      <c r="A3" s="0">
+        <v>0</v>
       </c>
-      <c r="B3" s="0">
-        <v>6000</v>
+      <c r="B3" s="0" t="s">
+        <v>7</v>
       </c>
       <c r="C3" s="0">
-        <v>60</v>
+        <v>5400</v>
       </c>
       <c r="D3" s="0">
-        <v>5940</v>
+        <v>5000</v>
       </c>
-      <c r="E3" s="0">
-        <v>940</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>7</v>
+      <c r="E3" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="s">
-        <v>6</v>
+      <c r="A4" s="0">
+        <v>0</v>
       </c>
-      <c r="B4" s="0">
-        <v>5000</v>
+      <c r="B4" s="0" t="s">
+        <v>9</v>
       </c>
       <c r="C4" s="0">
-        <v>50</v>
+        <v>4500</v>
       </c>
       <c r="D4" s="0">
-        <v>4950</v>
+        <v>4300</v>
       </c>
-      <c r="E4" s="0">
-        <v>950</v>
+      <c r="E4" s="0" t="s">
+        <v>10</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>8</v>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>43934.849675324076</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="0">
+        <v>5400</v>
+      </c>
+      <c r="D5" s="0">
+        <v>5400</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>